<commit_message>
chg: Updated with ordnance usage from D12.1
</commit_message>
<xml_diff>
--- a/MISSION INFORMATION/OPAR Ordnance CVN.xlsx
+++ b/MISSION INFORMATION/OPAR Ordnance CVN.xlsx
@@ -223,9 +223,6 @@
     <t>D16.1</t>
   </si>
   <si>
-    <t>D16.2</t>
-  </si>
-  <si>
     <t>D8</t>
   </si>
   <si>
@@ -245,6 +242,9 @@
   </si>
   <si>
     <t>DDG 2</t>
+  </si>
+  <si>
+    <t>Split frmo CV</t>
   </si>
 </sst>
 </file>
@@ -673,7 +673,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="5"/>
@@ -860,63 +860,6 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -945,6 +888,69 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -982,7 +988,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1150,7 +1156,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1525,7 +1531,7 @@
   <dimension ref="A1:V23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1552,17 +1558,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="92" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="93"/>
+      <c r="C1" s="96" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="98" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="78" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" s="80" t="s">
-        <v>67</v>
-      </c>
-      <c r="E1" s="80" t="s">
+      <c r="E1" s="98" t="s">
         <v>44</v>
       </c>
       <c r="F1" s="39"/>
@@ -1571,45 +1577,47 @@
       <c r="I1" s="39"/>
       <c r="J1" s="39"/>
       <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
+      <c r="L1" s="109" t="s">
+        <v>71</v>
+      </c>
       <c r="M1" s="39"/>
       <c r="N1" s="39"/>
       <c r="O1" s="39"/>
       <c r="P1" s="39"/>
-      <c r="Q1" s="81" t="s">
+      <c r="Q1" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="81"/>
-      <c r="S1" s="81"/>
-      <c r="T1" s="81"/>
-      <c r="U1" s="81"/>
-      <c r="V1" s="83" t="s">
-        <v>55</v>
+      <c r="R1" s="99"/>
+      <c r="S1" s="99"/>
+      <c r="T1" s="99"/>
+      <c r="U1" s="99"/>
+      <c r="V1" s="90" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="39.75" customHeight="1">
-      <c r="A2" s="76"/>
-      <c r="B2" s="77"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
+      <c r="A2" s="94"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
       <c r="F2" s="40"/>
       <c r="G2" s="40"/>
       <c r="H2" s="40"/>
       <c r="I2" s="40"/>
       <c r="J2" s="40"/>
       <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
+      <c r="L2" s="110"/>
       <c r="M2" s="40"/>
       <c r="N2" s="40"/>
       <c r="O2" s="40"/>
       <c r="P2" s="40"/>
-      <c r="Q2" s="82"/>
-      <c r="R2" s="82"/>
-      <c r="S2" s="82"/>
-      <c r="T2" s="82"/>
-      <c r="U2" s="82"/>
-      <c r="V2" s="84"/>
+      <c r="Q2" s="100"/>
+      <c r="R2" s="100"/>
+      <c r="S2" s="100"/>
+      <c r="T2" s="100"/>
+      <c r="U2" s="100"/>
+      <c r="V2" s="91"/>
     </row>
     <row r="3" spans="1:22" ht="15.75" customHeight="1" thickBot="1">
       <c r="A3" s="41" t="s">
@@ -1619,7 +1627,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="43" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D3" s="44"/>
       <c r="E3" s="44"/>
@@ -1641,35 +1649,33 @@
       <c r="K3" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="L3" s="46" t="s">
+      <c r="L3" s="46"/>
+      <c r="M3" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="M3" s="46" t="s">
+      <c r="N3" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="N3" s="46" t="s">
+      <c r="O3" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="O3" s="46" t="s">
+      <c r="P3" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="P3" s="46" t="s">
+      <c r="Q3" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="Q3" s="46" t="s">
+      <c r="R3" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="R3" s="46" t="s">
+      <c r="S3" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="S3" s="46" t="s">
+      <c r="T3" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="T3" s="46" t="s">
+      <c r="U3" s="46" t="s">
         <v>63</v>
-      </c>
-      <c r="U3" s="46" t="s">
-        <v>64</v>
       </c>
       <c r="V3" s="47" t="s">
         <v>1</v>
@@ -1703,7 +1709,7 @@
       <c r="S4" s="53"/>
       <c r="T4" s="53"/>
       <c r="U4" s="53"/>
-      <c r="V4" s="97">
+      <c r="V4" s="78">
         <f t="shared" ref="V4:V23" si="0">SUM(C4:E4)-SUM(F4:U4)</f>
         <v>47</v>
       </c>
@@ -1998,7 +2004,9 @@
       <c r="L12" s="52">
         <v>33</v>
       </c>
-      <c r="M12" s="52"/>
+      <c r="M12" s="52">
+        <v>1</v>
+      </c>
       <c r="N12" s="60"/>
       <c r="O12" s="52"/>
       <c r="P12" s="52"/>
@@ -2009,7 +2017,7 @@
       <c r="U12" s="53"/>
       <c r="V12" s="72">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:22">
@@ -2123,7 +2131,9 @@
       <c r="L15" s="57">
         <v>46</v>
       </c>
-      <c r="M15" s="57"/>
+      <c r="M15" s="57">
+        <v>2</v>
+      </c>
       <c r="N15" s="57"/>
       <c r="O15" s="57"/>
       <c r="P15" s="57"/>
@@ -2134,7 +2144,7 @@
       <c r="U15" s="58"/>
       <c r="V15" s="72">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:22">
@@ -2295,69 +2305,69 @@
     </row>
     <row r="20" spans="1:22" ht="11.25" customHeight="1" thickBot="1">
       <c r="N20" s="1"/>
-      <c r="V20" s="96"/>
+      <c r="V20" s="77"/>
     </row>
     <row r="21" spans="1:22">
-      <c r="A21" s="99" t="s">
+      <c r="A21" s="80" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="81" t="s">
         <v>68</v>
       </c>
-      <c r="B21" s="100" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" s="101">
+      <c r="C21" s="82">
         <v>20</v>
       </c>
-      <c r="D21" s="101"/>
-      <c r="E21" s="101"/>
-      <c r="F21" s="101"/>
-      <c r="G21" s="101"/>
-      <c r="H21" s="101"/>
-      <c r="I21" s="101"/>
-      <c r="J21" s="101"/>
-      <c r="K21" s="101"/>
-      <c r="L21" s="101"/>
-      <c r="M21" s="101"/>
-      <c r="N21" s="102"/>
-      <c r="O21" s="101"/>
-      <c r="P21" s="101"/>
-      <c r="Q21" s="101"/>
-      <c r="R21" s="101"/>
-      <c r="S21" s="101"/>
-      <c r="T21" s="101"/>
-      <c r="U21" s="107"/>
-      <c r="V21" s="98">
+      <c r="D21" s="82"/>
+      <c r="E21" s="82"/>
+      <c r="F21" s="82"/>
+      <c r="G21" s="82"/>
+      <c r="H21" s="82"/>
+      <c r="I21" s="82"/>
+      <c r="J21" s="82"/>
+      <c r="K21" s="82"/>
+      <c r="L21" s="82"/>
+      <c r="M21" s="82"/>
+      <c r="N21" s="83"/>
+      <c r="O21" s="82"/>
+      <c r="P21" s="82"/>
+      <c r="Q21" s="82"/>
+      <c r="R21" s="82"/>
+      <c r="S21" s="82"/>
+      <c r="T21" s="82"/>
+      <c r="U21" s="88"/>
+      <c r="V21" s="79">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:22">
       <c r="A22" s="48" t="s">
-        <v>68</v>
-      </c>
-      <c r="B22" s="93" t="s">
-        <v>70</v>
-      </c>
-      <c r="C22" s="94">
+        <v>67</v>
+      </c>
+      <c r="B22" s="74" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="75">
         <v>10</v>
       </c>
-      <c r="D22" s="94"/>
-      <c r="E22" s="94"/>
-      <c r="F22" s="94"/>
-      <c r="G22" s="94"/>
-      <c r="H22" s="94"/>
-      <c r="I22" s="94"/>
-      <c r="J22" s="94"/>
-      <c r="K22" s="94"/>
-      <c r="L22" s="94"/>
-      <c r="M22" s="94"/>
-      <c r="N22" s="95"/>
-      <c r="O22" s="94"/>
-      <c r="P22" s="94"/>
-      <c r="Q22" s="94"/>
-      <c r="R22" s="94"/>
-      <c r="S22" s="94"/>
-      <c r="T22" s="94"/>
-      <c r="U22" s="106"/>
+      <c r="D22" s="75"/>
+      <c r="E22" s="75"/>
+      <c r="F22" s="75"/>
+      <c r="G22" s="75"/>
+      <c r="H22" s="75"/>
+      <c r="I22" s="75"/>
+      <c r="J22" s="75"/>
+      <c r="K22" s="75"/>
+      <c r="L22" s="75"/>
+      <c r="M22" s="75"/>
+      <c r="N22" s="76"/>
+      <c r="O22" s="75"/>
+      <c r="P22" s="75"/>
+      <c r="Q22" s="75"/>
+      <c r="R22" s="75"/>
+      <c r="S22" s="75"/>
+      <c r="T22" s="75"/>
+      <c r="U22" s="87"/>
       <c r="V22" s="72">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2365,45 +2375,46 @@
     </row>
     <row r="23" spans="1:22" ht="15.75" thickBot="1">
       <c r="A23" s="65" t="s">
-        <v>68</v>
-      </c>
-      <c r="B23" s="103" t="s">
-        <v>71</v>
-      </c>
-      <c r="C23" s="104">
+        <v>67</v>
+      </c>
+      <c r="B23" s="84" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="85">
         <v>10</v>
       </c>
-      <c r="D23" s="104"/>
-      <c r="E23" s="104"/>
-      <c r="F23" s="104"/>
-      <c r="G23" s="104"/>
-      <c r="H23" s="104"/>
-      <c r="I23" s="104"/>
-      <c r="J23" s="104"/>
-      <c r="K23" s="104"/>
-      <c r="L23" s="104"/>
-      <c r="M23" s="104"/>
-      <c r="N23" s="105"/>
-      <c r="O23" s="104"/>
-      <c r="P23" s="104"/>
-      <c r="Q23" s="104"/>
-      <c r="R23" s="104"/>
-      <c r="S23" s="104"/>
-      <c r="T23" s="104"/>
-      <c r="U23" s="108"/>
+      <c r="D23" s="85"/>
+      <c r="E23" s="85"/>
+      <c r="F23" s="85"/>
+      <c r="G23" s="85"/>
+      <c r="H23" s="85"/>
+      <c r="I23" s="85"/>
+      <c r="J23" s="85"/>
+      <c r="K23" s="85"/>
+      <c r="L23" s="85"/>
+      <c r="M23" s="85"/>
+      <c r="N23" s="86"/>
+      <c r="O23" s="85"/>
+      <c r="P23" s="85"/>
+      <c r="Q23" s="85"/>
+      <c r="R23" s="85"/>
+      <c r="S23" s="85"/>
+      <c r="T23" s="85"/>
+      <c r="U23" s="89"/>
       <c r="V23" s="73">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="V1:V2"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="Q1:U2"/>
+    <mergeCell ref="L1:L2"/>
   </mergeCells>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -2438,13 +2449,13 @@
     <row r="1" spans="1:22" ht="15" customHeight="1">
       <c r="A1" s="7"/>
       <c r="B1" s="8"/>
-      <c r="C1" s="89" t="s">
+      <c r="C1" s="105" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="92" t="s">
+      <c r="D1" s="108" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="91" t="s">
+      <c r="E1" s="107" t="s">
         <v>44</v>
       </c>
       <c r="F1" s="8"/>
@@ -2458,23 +2469,23 @@
       <c r="N1" s="8"/>
       <c r="O1" s="8"/>
       <c r="P1" s="8"/>
-      <c r="Q1" s="87" t="s">
+      <c r="Q1" s="103" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="87"/>
-      <c r="S1" s="87"/>
-      <c r="T1" s="87"/>
-      <c r="U1" s="87"/>
-      <c r="V1" s="85" t="s">
+      <c r="R1" s="103"/>
+      <c r="S1" s="103"/>
+      <c r="T1" s="103"/>
+      <c r="U1" s="103"/>
+      <c r="V1" s="101" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="69.75" customHeight="1">
       <c r="A2" s="9"/>
       <c r="B2" s="34"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="91"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="107"/>
       <c r="F2" s="34"/>
       <c r="G2" s="34"/>
       <c r="H2" s="34"/>
@@ -2486,12 +2497,12 @@
       <c r="N2" s="34"/>
       <c r="O2" s="34"/>
       <c r="P2" s="34"/>
-      <c r="Q2" s="88"/>
-      <c r="R2" s="88"/>
-      <c r="S2" s="88"/>
-      <c r="T2" s="88"/>
-      <c r="U2" s="88"/>
-      <c r="V2" s="86"/>
+      <c r="Q2" s="104"/>
+      <c r="R2" s="104"/>
+      <c r="S2" s="104"/>
+      <c r="T2" s="104"/>
+      <c r="U2" s="104"/>
+      <c r="V2" s="102"/>
     </row>
     <row r="3" spans="1:22" ht="15.75" thickBot="1">
       <c r="A3" s="10" t="s">

</xml_diff>